<commit_message>
Fixed column name in xls
</commit_message>
<xml_diff>
--- a/xls/dados.xlsx
+++ b/xls/dados.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="38120" windowHeight="19740" tabRatio="869"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="38120" windowHeight="19740" tabRatio="869" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tabela 1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="154">
   <si>
     <t>Total</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>60 e mais</t>
-  </si>
-  <si>
-    <t>Residência</t>
   </si>
   <si>
     <t>Masculino</t>
@@ -1230,7 +1227,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B16" sqref="A16:B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -1243,7 +1242,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1264,10 +1263,10 @@
     </row>
     <row r="2" spans="1:19" s="87" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="85" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="85" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="85" t="s">
         <v>2</v>
@@ -1276,22 +1275,22 @@
         <v>1</v>
       </c>
       <c r="E2" s="85" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="85" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="85" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="I2" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="I2" s="85" t="s">
+      <c r="J2" s="86" t="s">
         <v>104</v>
-      </c>
-      <c r="J2" s="86" t="s">
-        <v>105</v>
       </c>
       <c r="L2" s="88"/>
       <c r="M2" s="89"/>
@@ -2587,7 +2586,7 @@
     </row>
     <row r="38" spans="1:19" ht="15" customHeight="1">
       <c r="E38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2615,21 +2614,21 @@
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="D2" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
@@ -3104,24 +3103,24 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
@@ -3692,54 +3691,54 @@
   <sheetData>
     <row r="1" spans="1:16" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="K2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>134</v>
-      </c>
       <c r="O2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>0</v>
@@ -5370,38 +5369,38 @@
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I1" s="91"/>
       <c r="J1" s="91"/>
     </row>
     <row r="2" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>120</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>0</v>
@@ -6462,21 +6461,21 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>0</v>
@@ -7032,17 +7031,17 @@
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -7073,18 +7072,18 @@
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>0</v>
@@ -7543,12 +7542,12 @@
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1">
       <c r="A37" s="49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -7586,48 +7585,48 @@
   <sheetData>
     <row r="1" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="E2" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="F2" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="F2" s="48" t="s">
-        <v>144</v>
-      </c>
       <c r="G2" s="50" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="I2" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="J2" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="K2" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="L2" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="50" t="s">
-        <v>45</v>
-      </c>
       <c r="M2" s="50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N2" s="50" t="s">
         <v>0</v>
@@ -9058,7 +9057,7 @@
     </row>
     <row r="36" spans="1:14" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="33"/>
       <c r="F36" s="33"/>
@@ -9066,13 +9065,13 @@
     </row>
     <row r="37" spans="1:14" ht="15" customHeight="1">
       <c r="A37" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N37" s="52"/>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1">
       <c r="A38" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M38" s="33"/>
       <c r="N38" s="52"/>
@@ -9084,18 +9083,18 @@
     </row>
     <row r="40" spans="1:14" ht="15" customHeight="1">
       <c r="A40" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N40" s="52"/>
     </row>
     <row r="41" spans="1:14" ht="15" customHeight="1">
       <c r="A41" s="54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1">
       <c r="A42" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1">
@@ -9131,24 +9130,24 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="D2" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>146</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>0</v>
@@ -9804,14 +9803,14 @@
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" s="47"/>
       <c r="E36" s="55"/>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="59" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B38" s="56"/>
       <c r="C38" s="56"/>
@@ -9829,7 +9828,7 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" s="59" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="56"/>
       <c r="C40" s="56"/>
@@ -9847,7 +9846,7 @@
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1">
       <c r="A42" s="59" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B42" s="56"/>
       <c r="C42" s="56"/>
@@ -9865,7 +9864,7 @@
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1">
       <c r="A44" s="59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="56"/>
       <c r="C44" s="56"/>
@@ -9883,7 +9882,7 @@
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1">
       <c r="A46" s="59" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B46" s="58"/>
       <c r="C46" s="58"/>
@@ -9893,7 +9892,7 @@
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1">
       <c r="A47" s="59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" s="58"/>
       <c r="C47" s="58"/>
@@ -9903,7 +9902,7 @@
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1">
       <c r="A48" s="59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="56"/>
       <c r="C48" s="56"/>
@@ -9926,7 +9925,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -9945,39 +9946,39 @@
   <sheetData>
     <row r="1" spans="1:11" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>0</v>
@@ -11132,7 +11133,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="78"/>
       <c r="C1" s="78"/>
@@ -11141,19 +11142,19 @@
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="70" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="70" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" s="70" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
@@ -11696,12 +11697,12 @@
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1">
       <c r="A38" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B38" s="80"/>
       <c r="C38" s="80"/>
@@ -11717,7 +11718,7 @@
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1">
       <c r="A40" s="61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="80"/>
       <c r="C40" s="80"/>
@@ -11733,7 +11734,7 @@
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1">
       <c r="A42" s="61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" s="80"/>
       <c r="C42" s="80"/>
@@ -11749,7 +11750,7 @@
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1">
       <c r="A44" s="61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="80"/>
       <c r="C44" s="80"/>
@@ -11758,7 +11759,7 @@
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1">
       <c r="A45" s="61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" s="80"/>
       <c r="C45" s="80"/>
@@ -11767,7 +11768,7 @@
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1">
       <c r="A46" s="61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B46" s="80"/>
       <c r="C46" s="80"/>
@@ -11802,7 +11803,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -11819,7 +11820,7 @@
     </row>
     <row r="2" spans="1:13" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>4</v>
@@ -13208,48 +13209,48 @@
   <sheetData>
     <row r="1" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>57</v>
-      </c>
       <c r="M2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N2" s="8" t="s">
         <v>0</v>
@@ -14712,12 +14713,12 @@
     </row>
     <row r="36" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1">
       <c r="A38" s="67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="65"/>
       <c r="C38" s="65"/>
@@ -14735,7 +14736,7 @@
     </row>
     <row r="39" spans="1:14" ht="15" customHeight="1">
       <c r="A39" s="67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B39" s="65"/>
       <c r="C39" s="65"/>
@@ -14769,7 +14770,7 @@
     </row>
     <row r="41" spans="1:14" ht="15" customHeight="1">
       <c r="A41" s="67" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" s="65"/>
       <c r="C41" s="65"/>
@@ -14787,7 +14788,7 @@
     </row>
     <row r="42" spans="1:14" ht="15" customHeight="1">
       <c r="A42" s="67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" s="65"/>
       <c r="C42" s="65"/>
@@ -14805,7 +14806,7 @@
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1">
       <c r="A43" s="67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="65"/>
       <c r="C43" s="65"/>
@@ -14849,24 +14850,24 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="E2" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>0</v>
@@ -15519,12 +15520,12 @@
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="63" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B38" s="62"/>
       <c r="C38" s="62"/>
@@ -15542,7 +15543,7 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" s="63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="62"/>
       <c r="C40" s="62"/>
@@ -15560,7 +15561,7 @@
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1">
       <c r="A42" s="63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B42" s="62"/>
       <c r="C42" s="62"/>
@@ -15578,7 +15579,7 @@
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1">
       <c r="A44" s="63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1">
@@ -15586,17 +15587,17 @@
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1">
       <c r="A46" s="63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1">
       <c r="A47" s="63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1">
       <c r="A48" s="63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -15613,7 +15614,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40:F41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -15629,39 +15632,39 @@
   <sheetData>
     <row r="1" spans="1:11" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>0</v>
@@ -16810,7 +16813,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -16821,22 +16824,22 @@
     </row>
     <row r="2" spans="1:7" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="E2" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="27" t="s">
+      <c r="F2" s="27" t="s">
         <v>109</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>110</v>
       </c>
       <c r="G2" s="27" t="s">
         <v>0</v>
@@ -17603,7 +17606,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="21" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -17611,13 +17614,13 @@
     </row>
     <row r="2" spans="1:4" s="21" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>17</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>0</v>
@@ -18101,27 +18104,27 @@
   <sheetData>
     <row r="1" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="D2" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>20</v>
       </c>
       <c r="G2" s="28" t="s">
         <v>0</v>
@@ -18889,7 +18892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -18903,25 +18906,25 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" s="36"/>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B2" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
@@ -19470,7 +19473,7 @@
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -19498,7 +19501,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -19509,25 +19512,25 @@
     </row>
     <row r="2" spans="1:7" ht="12">
       <c r="A2" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>64</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
@@ -20277,7 +20280,7 @@
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1">
       <c r="A36" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B36" s="38"/>
       <c r="C36" s="38"/>
@@ -20288,7 +20291,7 @@
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1">
       <c r="A37" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="38"/>
       <c r="C37" s="38"/>
@@ -20324,39 +20327,39 @@
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="83" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="83" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="83" t="s">
+      <c r="D2" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="83" t="s">
+      <c r="E2" s="83" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="83" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="83" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="83" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="83" t="s">
+      <c r="H2" s="83" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="83" t="s">
+      <c r="I2" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="83" t="s">
+      <c r="J2" s="83" t="s">
         <v>120</v>
-      </c>
-      <c r="J2" s="83" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">
@@ -21408,39 +21411,39 @@
   <sheetData>
     <row r="1" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>78</v>
-      </c>
       <c r="D2" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="F2" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="H2" s="28" t="s">
+      <c r="J2" s="28" t="s">
         <v>124</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1">

</xml_diff>